<commit_message>
Documento de requisitos secao 3 e documento de transacoes
</commit_message>
<xml_diff>
--- a/documentos/SRP-Transacoes.xlsx
+++ b/documentos/SRP-Transacoes.xlsx
@@ -131,6 +131,32 @@
         </r>
       </text>
     </comment>
+    <comment ref="F2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Rafael Vargas:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Listagem Específica 1</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="F14" authorId="0">
       <text>
         <r>
@@ -153,37 +179,271 @@
             <family val="0"/>
             <charset val="1"/>
           </rPr>
+          <t xml:space="preserve">Listagem Específica 1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Rafael Vargas:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Listagem Específica 5</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Rafael Vargas:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Listagem Específica 2</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Rafael Vargas:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Listagem Específica 2</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Rafael Vargas:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Listagem Específica 6</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Rafael Vargas:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Listagem Específica 3</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Rafael Vargas:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Listagem Específica 3</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Rafael Vargas:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Listagem Específica 7</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Rafael Vargas:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
           <t xml:space="preserve">Regra de Negócio 1</t>
         </r>
       </text>
     </comment>
-    <comment ref="F20" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b val="true"/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Rafael Vargas:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Listagem Específica 5</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G14" authorId="0">
+    <comment ref="I14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Rafael Vargas:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Regra de Negócio 1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Rafael Vargas:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Listagem Específica 8</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -209,33 +469,59 @@
         </r>
       </text>
     </comment>
-    <comment ref="G20" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b val="true"/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Rafael Vargas:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Listagem Específica 6</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H14" authorId="0">
+    <comment ref="J14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Rafael Vargas:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Regra de Negócio 2</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Rafael Vargas:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Listagem Específica 9</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -261,81 +547,29 @@
         </r>
       </text>
     </comment>
-    <comment ref="H20" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b val="true"/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Rafael Vargas:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Listagem Específica 7</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I20" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b val="true"/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Rafael Vargas:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Listagem Específica 8</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J20" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b val="true"/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Rafael Vargas:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Listagem Específica 9</t>
+    <comment ref="K14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Rafael Vargas:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Regra de Negócio 3</t>
         </r>
       </text>
     </comment>
@@ -370,7 +604,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t xml:space="preserve">Manutenção de Cadastros</t>
   </si>
@@ -387,6 +621,24 @@
     <t xml:space="preserve">Listar Todos</t>
   </si>
   <si>
+    <t xml:space="preserve">List. Espec. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List. Espec. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List. Espec. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regra Neg. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regra Neg. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regra Neg. 3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Administrador</t>
   </si>
   <si>
@@ -417,15 +669,6 @@
     <t xml:space="preserve">Processo de Negócio</t>
   </si>
   <si>
-    <t xml:space="preserve">Regra Neg. 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regra Neg. 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regra Neg. 3</t>
-  </si>
-  <si>
     <t xml:space="preserve">Recarga</t>
   </si>
   <si>
@@ -433,18 +676,6 @@
   </si>
   <si>
     <t xml:space="preserve">Saque</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proces</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List. Espec. 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List. Espec. 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List. Espec. 3</t>
   </si>
   <si>
     <t xml:space="preserve">List. Espec. 4</t>
@@ -678,18 +909,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="topLeft" activeCell="L21" activeCellId="0" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.42"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="6" style="0" width="11.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.68"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -721,16 +953,28 @@
       <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>1</v>
@@ -753,7 +997,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>1</v>
@@ -770,13 +1014,15 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+      <c r="I4" s="3" t="n">
+        <v>1</v>
+      </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>1</v>
@@ -793,13 +1039,15 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="I5" s="3" t="n">
+        <v>1</v>
+      </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>1</v>
@@ -822,7 +1070,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3" t="n">
         <v>1</v>
@@ -845,7 +1093,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B8" s="3" t="n">
         <v>1</v>
@@ -868,7 +1116,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B9" s="3" t="n">
         <v>1</v>
@@ -891,7 +1139,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B10" s="3" t="n">
         <v>1</v>
@@ -914,7 +1162,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B11" s="3" t="n">
         <v>1</v>
@@ -950,7 +1198,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -978,21 +1226,27 @@
         <v>4</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B15" s="3" t="n">
         <v>1</v>
@@ -1009,13 +1263,19 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
+      <c r="I15" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J15" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" s="3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B16" s="3" t="n">
         <v>1</v>
@@ -1032,13 +1292,17 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
+      <c r="I16" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16" s="3" t="n">
+        <v>1</v>
+      </c>
       <c r="K16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B17" s="3" t="n">
         <v>1</v>
@@ -1055,7 +1319,9 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+      <c r="I17" s="3" t="n">
+        <v>1</v>
+      </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
     </row>
@@ -1074,7 +1340,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1090,37 +1356,37 @@
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="G20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="H20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="I20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="J20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="K20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K20" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1135,13 +1401,15 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="4" t="n">
         <f aca="false">COUNT(B3:K12,B15:K18,B21:K21)</f>
-        <v>48</v>
-      </c>
-    </row>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:K1"/>
@@ -1170,7 +1438,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.68"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1193,7 +1464,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.68"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Correção das iterações e remoção do conceito de Linha
</commit_message>
<xml_diff>
--- a/documentos/SRP-Transacoes.xlsx
+++ b/documentos/SRP-Transacoes.xlsx
@@ -170,7 +170,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F14" authorId="0">
+    <comment ref="F13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -194,7 +194,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G14" authorId="0">
+    <comment ref="G13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -218,7 +218,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H14" authorId="0">
+    <comment ref="H13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -242,7 +242,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I14" authorId="0">
+    <comment ref="I13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -266,7 +266,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J14" authorId="0">
+    <comment ref="J13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -290,7 +290,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K14" authorId="0">
+    <comment ref="K13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -314,7 +314,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B20" authorId="0">
+    <comment ref="B19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -338,7 +338,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C20" authorId="0">
+    <comment ref="C19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -362,7 +362,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D20" authorId="0">
+    <comment ref="D19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -386,7 +386,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E20" authorId="0">
+    <comment ref="E19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -410,7 +410,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F20" authorId="0">
+    <comment ref="F19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -434,7 +434,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G20" authorId="0">
+    <comment ref="G19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -458,7 +458,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H20" authorId="0">
+    <comment ref="H19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -482,7 +482,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I20" authorId="0">
+    <comment ref="I19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -506,7 +506,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J20" authorId="0">
+    <comment ref="J19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -530,7 +530,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K20" authorId="0">
+    <comment ref="K19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -559,7 +559,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
   <si>
     <t>Manutenção de Cadastros</t>
   </si>
@@ -616,9 +616,6 @@
   </si>
   <si>
     <t>Empresa</t>
-  </si>
-  <si>
-    <t>Linha</t>
   </si>
   <si>
     <t>Processo de Negócio</t>
@@ -734,14 +731,14 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -836,7 +833,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -879,7 +876,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -922,7 +919,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -965,7 +962,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1008,7 +1005,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1051,7 +1048,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1094,7 +1091,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1137,7 +1134,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1180,7 +1177,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1223,7 +1220,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1266,7 +1263,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1309,7 +1306,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1352,7 +1349,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1395,7 +1392,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1438,7 +1435,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1481,7 +1478,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1524,7 +1521,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1567,7 +1564,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1610,7 +1607,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1653,7 +1650,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1696,7 +1693,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1739,12 +1736,958 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="1026" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1089" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1088" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1087" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1086" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1085" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1084" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1083" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1082" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1081" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1080" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1079" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1078" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1077" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1076" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1075" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1074" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1073" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1072" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1071" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1070" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1069" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="_x0000_t202" hidden="1"/>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2062,10 +3005,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2078,504 +3021,481 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3">
-        <v>1</v>
-      </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3">
-        <v>1</v>
-      </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3">
-        <v>1</v>
-      </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3">
-        <v>1</v>
-      </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="3">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3">
-        <v>1</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="3">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3">
-        <v>1</v>
-      </c>
-      <c r="E7" s="3">
-        <v>1</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="3">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3">
-        <v>1</v>
-      </c>
-      <c r="E8" s="3">
-        <v>1</v>
-      </c>
-      <c r="F8" s="3">
-        <v>1</v>
-      </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="3">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="3">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1</v>
-      </c>
-      <c r="D10" s="3">
-        <v>1</v>
-      </c>
-      <c r="E10" s="3">
-        <v>1</v>
-      </c>
-      <c r="F10" s="3">
-        <v>1</v>
-      </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="3">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3">
-        <v>1</v>
-      </c>
-      <c r="D11" s="3">
-        <v>1</v>
-      </c>
-      <c r="E11" s="3">
-        <v>1</v>
-      </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+      <c r="A12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>10</v>
+      <c r="A14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2">
+        <v>1</v>
+      </c>
+      <c r="J14" s="2">
+        <v>1</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="3">
-        <v>1</v>
-      </c>
-      <c r="C15" s="3">
-        <v>1</v>
-      </c>
-      <c r="D15" s="3">
-        <v>1</v>
-      </c>
-      <c r="E15" s="3">
-        <v>1</v>
-      </c>
-      <c r="F15" s="3">
-        <v>1</v>
-      </c>
-      <c r="G15" s="3">
-        <v>1</v>
-      </c>
-      <c r="H15" s="3">
-        <v>1</v>
-      </c>
-      <c r="I15" s="3">
-        <v>1</v>
-      </c>
-      <c r="J15" s="3">
-        <v>1</v>
-      </c>
-      <c r="K15" s="3">
-        <v>1</v>
-      </c>
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2">
+        <v>1</v>
+      </c>
+      <c r="J15" s="2">
+        <v>1</v>
+      </c>
+      <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="3">
-        <v>1</v>
-      </c>
-      <c r="C16" s="3">
-        <v>1</v>
-      </c>
-      <c r="D16" s="3">
-        <v>1</v>
-      </c>
-      <c r="E16" s="3">
-        <v>1</v>
-      </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3">
-        <v>1</v>
-      </c>
-      <c r="J16" s="3">
-        <v>1</v>
-      </c>
-      <c r="K16" s="3"/>
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2">
+        <v>1</v>
+      </c>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="3">
-        <v>1</v>
-      </c>
-      <c r="C17" s="3">
-        <v>1</v>
-      </c>
-      <c r="D17" s="3">
-        <v>1</v>
-      </c>
-      <c r="E17" s="3">
-        <v>1</v>
-      </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3">
-        <v>1</v>
-      </c>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
+      <c r="A18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
-      <c r="B20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K20" s="2" t="s">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="4">
-        <f>COUNT(B3:K12,B15:K18,B21:K21)</f>
-        <v>61</v>
+      <c r="B22" s="3">
+        <f>COUNT(B3:K11,B14:K17,B20:K20)</f>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A13:K13"/>
-    <mergeCell ref="A19:K19"/>
+    <mergeCell ref="A12:K12"/>
+    <mergeCell ref="A18:K18"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Novos requisitos de listagem e atualização do cronograma
</commit_message>
<xml_diff>
--- a/documentos/SRP-Transacoes.xlsx
+++ b/documentos/SRP-Transacoes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="473"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
+    <author>João Victor Costa Araujo</author>
   </authors>
   <commentList>
     <comment ref="F2" authorId="0">
@@ -170,6 +171,78 @@
         </r>
       </text>
     </comment>
+    <comment ref="F4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>João Victor Costa Araujo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Listar quantidades de Clientes (Por empresa)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>João Victor Costa Araujo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Verificar se já existe um cliente com o mesmo CPF</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I5" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>João Victor Costa Araujo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Verificar se já existe um usuário utilizando o mesmo cartão inteligente</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="F13" authorId="0">
       <text>
         <r>
@@ -311,6 +384,246 @@
             <charset val="1"/>
           </rPr>
           <t>Regra de Negócio 3</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F14" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>João Victor Costa Araujo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Listar totais e quantidades de recargas nas Empresas (data início e data término)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G14" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>João Victor Costa Araujo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Listar totais e quantidades de recargas nas Cidades (Por UF, data início e data término)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H14" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>João Victor Costa Araujo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Listar recargas (Por cliente, data início e data término)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I14" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>João Victor Costa Araujo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Verificar se a soma entre os valores das recargas pendentes e a carteira do usuário não ultrapassa R$ 200,00.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J14" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>João Victor Costa Araujo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Verificar se o usuário possui 20 recargas pendentes</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K14" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>João Victor Costa Araujo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Verificar se existe algum saque pendente</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I15" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>João Victor Costa Araujo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Verificar se o usuário já possui três agendamentos</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J15" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>João Victor Costa Araujo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Verificar se já existe algum outro agendamento configurado para o mesmo dia</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F16" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>João Victor Costa Araujo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Listar saques (Por cliente, data início e data término)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I16" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>João Victor Costa Araujo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Verificar se já foi realizado algum saque no dia</t>
         </r>
       </text>
     </comment>
@@ -658,7 +971,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -684,6 +997,19 @@
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
@@ -2715,6 +3041,1898 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1121" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1120" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1119" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1118" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1117" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1116" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1115" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1114" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1113" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1112" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1111" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1110" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1109" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1108" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1107" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1106" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1105" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1104" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1103" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1102" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1101" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1100" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3008,7 +5226,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3107,7 +5325,9 @@
       <c r="E4" s="2">
         <v>1</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2">
@@ -3203,9 +5423,7 @@
       <c r="E8" s="2">
         <v>1</v>
       </c>
-      <c r="F8" s="2">
-        <v>1</v>
-      </c>
+      <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -3251,9 +5469,7 @@
       <c r="E10" s="2">
         <v>1</v>
       </c>
-      <c r="F10" s="2">
-        <v>1</v>
-      </c>
+      <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -3399,7 +5615,9 @@
       <c r="E16" s="2">
         <v>1</v>
       </c>
-      <c r="F16" s="2"/>
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2">

</xml_diff>

<commit_message>
Documento de requisitos: alteração nas regras de negócio do caso de uso de agendamento
</commit_message>
<xml_diff>
--- a/documentos/SRP-Transacoes.xlsx
+++ b/documentos/SRP-Transacoes.xlsx
@@ -552,30 +552,6 @@
           </rPr>
           <t xml:space="preserve">
 Verificar se o usuário já possui três agendamentos</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J15" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>João Victor Costa Araujo:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Verificar se já existe algum outro agendamento configurado para o mesmo dia</t>
         </r>
       </text>
     </comment>
@@ -4933,6 +4909,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1127" name="_x0000_t202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5594,9 +5613,7 @@
       <c r="I15" s="2">
         <v>1</v>
       </c>
-      <c r="J15" s="2">
-        <v>1</v>
-      </c>
+      <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -5706,7 +5723,7 @@
       </c>
       <c r="B22" s="3">
         <f>COUNT(B3:K11,B14:K17,B20:K20)</f>
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>